<commit_message>
Added pressure toggle web elements
Added pressure toggle web elements and excel files
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/PressureValues.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/PressureValues.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Raj\git\nordsonomu_automation\nordson.omu\src\test\java\com\nordson\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654E19B4-F7FB-4C94-9EEA-207B38BA4C17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="971" firstSheet="1" activeTab="7" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
+    <workbookView windowWidth="11448" windowHeight="2471" tabRatio="971" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="kpaMinMaxSameValues" sheetId="1" r:id="rId1"/>
@@ -22,34 +16,23 @@
     <sheet name="PSIMinMaxSameValues" sheetId="7" r:id="rId7"/>
     <sheet name="PSI_Min_Max_0_101" sheetId="8" r:id="rId8"/>
     <sheet name="PSI_Min_Max_0_100" sheetId="9" r:id="rId9"/>
+    <sheet name="PSIminRange" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
+  <oleSize ref="B1:C2"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
-    <t>Kpa min value</t>
+    <t>kpa min value</t>
   </si>
   <si>
     <t>kpa max value</t>
   </si>
   <si>
-    <t>kpa min value</t>
+    <t>Kpa min value</t>
   </si>
   <si>
     <t>BAR min value</t>
@@ -61,49 +44,197 @@
     <t>PSI min value</t>
   </si>
   <si>
-    <t>PSI max value</t>
+    <t>PSI  max value</t>
   </si>
   <si>
-    <t>PSI  max value</t>
+    <t>PSI max value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,41 +249,286 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF53A1B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="15">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -172,83 +548,332 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="49" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="49" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="49" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{19DFC39A-23B0-4ADC-AB54-D047D0C5623A}"/>
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Excel Built-in Normal" xfId="49"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFF53A1B"/>
-      <color rgb="FFEF6425"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="00F53A1B"/>
+      <color rgb="00EF6425"/>
+      <color rgb="00FFFFFF"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -297,7 +922,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -330,26 +955,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -382,23 +990,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,388 +1131,430 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E1DBC9-FCF4-45E5-B4FD-5A6169F6B019}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.4444444444444" customWidth="1"/>
+    <col min="3" max="3" width="18.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="2:3">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="3">
+    <row r="2" spans="2:3">
+      <c r="B2" s="14">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="4">
+    <row r="3" spans="2:3">
+      <c r="B3" s="15">
         <v>0</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="15">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="4">
+    <row r="4" spans="2:3">
+      <c r="B4" s="15">
         <v>0</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="15">
         <v>689</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="3">
+    <row r="5" spans="2:3">
+      <c r="B5" s="14">
         <v>656</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="14">
         <v>690</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="3">
+    <row r="6" spans="2:3">
+      <c r="B6" s="14">
         <v>333</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="14">
         <v>345</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="17.1111111111111" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" s="3">
+        <v>96</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF66B099-76A0-4630-B7C5-6712EE2C5428}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="22.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:3">
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" s="14">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="C2" s="14">
         <v>691</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
+    <row r="3" spans="2:3">
+      <c r="B3" s="11">
         <v>655</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="11">
         <v>690</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="6">
+    <row r="4" spans="2:3">
+      <c r="B4" s="10">
         <v>656</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="10">
         <v>691</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4E0107-5920-4F1B-AA99-1A3D13CE0D5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="21.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="2:3">
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="7">
+    <row r="2" spans="2:3">
+      <c r="B2" s="13">
         <v>0</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="13">
         <v>690</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BDA572-95CB-4C0F-BFE9-D19F976A5730}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.4444444444444" customWidth="1"/>
+    <col min="3" max="3" width="24.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:3">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="6">
+    <row r="2" spans="2:3">
+      <c r="B2" s="10">
         <v>7</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="8">
+    <row r="3" spans="2:3">
+      <c r="B3" s="6">
         <v>0</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>0.34</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="8">
+    <row r="4" spans="2:3">
+      <c r="B4" s="6">
         <v>6.55</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>6.9</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
+    <row r="5" spans="2:3">
+      <c r="B5" s="10">
         <v>5.56</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="10">
         <v>5.57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A9D19F-96A2-4B1E-9CA4-FB24F8DEBCF5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="25.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:3">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="6">
+    <row r="2" spans="2:3">
+      <c r="B2" s="10">
         <v>1.9</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="10">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170A38D9-C444-4FC9-B2A6-34EAF4896CB1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="24.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:3">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="8">
+    <row r="2" spans="2:3">
+      <c r="B2" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="6">
         <v>6.9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F6A708-03CB-449A-A84B-E21AA5507797}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="29.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:3">
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="6">
+    <row r="2" spans="2:3">
+      <c r="B2" s="10">
         <v>50</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="10">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
+    <row r="3" spans="2:3">
+      <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+    <row r="4" spans="2:3">
+      <c r="B4" s="11">
         <v>95</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="11">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
+    <row r="5" spans="2:3">
+      <c r="B5" s="10">
         <v>0</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="10">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="6">
+    <row r="6" spans="2:3">
+      <c r="B6" s="10">
         <v>96</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="10">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7DF7BB-FD06-4419-854B-C831BB8AE32A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="30.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="2:3">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
       <c r="B2" s="9">
         <v>0</v>
       </c>
@@ -931,41 +1564,44 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACC4B9A-2110-4E2B-8390-C455D5AB778F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:3">
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="8">
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="6">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>